<commit_message>
Conclutions added to Resultados file
</commit_message>
<xml_diff>
--- a/Resultados/0) Resultados.xlsx
+++ b/Resultados/0) Resultados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1) Documentos\1) Universidad\Cátedra Lucha Colombiana contra la Corrupción\Codigo\Resultados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD6A4CE-5EB0-4431-B8ED-313BADA6ABD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD8CE87-1522-4CCD-AF29-9452046BEF51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-3375" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -670,9 +670,8 @@
     <xf numFmtId="2" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -700,8 +699,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1564,7 +1564,7 @@
   <dimension ref="B1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1574,391 +1574,391 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="20"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="21"/>
     </row>
     <row r="7" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24"/>
     </row>
     <row r="8" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17"/>
-      <c r="H9" s="15" t="s">
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
+      <c r="H9" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="18"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="20"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="21"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="21"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="20"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="20"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="21"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="20"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="21"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="20"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="21"/>
     </row>
     <row r="14" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="21"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="23"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="23"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="24"/>
     </row>
     <row r="15" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="18"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="20"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="20"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="20"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
     </row>
     <row r="20" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="21"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="23"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="24"/>
     </row>
     <row r="21" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="18"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="20"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="20"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="21"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="20"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="21"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="18"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="20"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="21"/>
     </row>
     <row r="27" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="21"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="23"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="24"/>
     </row>
     <row r="28" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="18"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="20"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="21"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="18"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="20"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="21"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="18"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="20"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="21"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B33" s="18"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="20"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="21"/>
     </row>
     <row r="34" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="21"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="23"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="24"/>
     </row>
     <row r="35" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="36" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="18"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B37" s="18"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="20"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="21"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B38" s="18"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="20"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="21"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B39" s="18"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="20"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="21"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B40" s="18"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="20"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="21"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B41" s="18"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="20"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="21"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B42" s="18"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="20"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="21"/>
     </row>
     <row r="43" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="21"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="23"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="24"/>
     </row>
     <row r="44" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="45" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="17"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="18"/>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B46" s="18"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="20"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="21"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B47" s="18"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="20"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="21"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B48" s="18"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="20"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="21"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B49" s="18"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="20"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="21"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B50" s="18"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="20"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="21"/>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B51" s="18"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="20"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="21"/>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B52" s="18"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="20"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="21"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B53" s="18"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="20"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="21"/>
     </row>
     <row r="54" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="21"/>
-      <c r="C54" s="22"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="22"/>
-      <c r="F54" s="23"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23"/>
+      <c r="F54" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2099,10 +2099,10 @@
         <f>AVERAGE(etha0_n0_5_iterations50_seed1[Error])</f>
         <v>11.667187499999994</v>
       </c>
-      <c r="H6" s="24"/>
-      <c r="I6" s="25"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="25"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="15"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="15"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -3827,22 +3827,22 @@
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="H7" s="14" t="s">
+      <c r="C7" s="25"/>
+      <c r="H7" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="N7" s="14" t="s">
+      <c r="I7" s="25"/>
+      <c r="N7" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="O7" s="14"/>
-      <c r="T7" s="14" t="s">
+      <c r="O7" s="25"/>
+      <c r="T7" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="U7" s="14"/>
+      <c r="U7" s="25"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
@@ -6026,18 +6026,18 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="H7" s="14" t="s">
+      <c r="C7" s="25"/>
+      <c r="H7" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="N7" s="14" t="s">
+      <c r="I7" s="25"/>
+      <c r="N7" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="O7" s="14"/>
+      <c r="O7" s="25"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
@@ -7757,22 +7757,22 @@
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="H7" s="14" t="s">
+      <c r="C7" s="25"/>
+      <c r="H7" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="N7" s="14" t="s">
+      <c r="I7" s="25"/>
+      <c r="N7" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="O7" s="14"/>
-      <c r="T7" s="14" t="s">
+      <c r="O7" s="25"/>
+      <c r="T7" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="U7" s="14"/>
+      <c r="U7" s="25"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
@@ -9956,18 +9956,18 @@
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="H7" s="14" t="s">
+      <c r="C7" s="25"/>
+      <c r="H7" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="N7" s="14" t="s">
+      <c r="I7" s="25"/>
+      <c r="N7" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="O7" s="14"/>
+      <c r="O7" s="25"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" t="s">

</xml_diff>